<commit_message>
typo fix for vercel Limit
</commit_message>
<xml_diff>
--- a/costs/Tech_costs.xlsx
+++ b/costs/Tech_costs.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tyler\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\tyler\projects\startup\design-and-architecture\costs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4708E8C-EEC3-4597-BD3E-13B3DC54D55A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE69CCC3-556A-42AF-9262-9C5F8A1F9999}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-24110" yWindow="-1470" windowWidth="24220" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -119,9 +119,6 @@
     <t>Rate/Limit</t>
   </si>
   <si>
-    <t>est. 10,000 month</t>
-  </si>
-  <si>
     <t>Free tier &amp; Annual pricing available</t>
   </si>
   <si>
@@ -147,6 +144,9 @@
   </si>
   <si>
     <t>N/A</t>
+  </si>
+  <si>
+    <t>est. 10,000 visitors month</t>
   </si>
 </sst>
 </file>
@@ -213,7 +213,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -222,9 +222,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -538,7 +535,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -567,7 +564,7 @@
       <c r="E1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>27</v>
       </c>
     </row>
@@ -575,7 +572,7 @@
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="5">
         <v>20</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -587,15 +584,15 @@
       <c r="E2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>28</v>
+      <c r="F2" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="5">
         <v>7</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -608,14 +605,14 @@
         <v>17</v>
       </c>
       <c r="F3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="5">
         <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -628,14 +625,14 @@
         <v>17</v>
       </c>
       <c r="F4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="5">
         <v>0</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -648,21 +645,21 @@
         <v>15</v>
       </c>
       <c r="F5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="5">
         <v>49</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>20</v>
@@ -675,7 +672,7 @@
       <c r="A7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="4">
         <f>229.99 / 12</f>
         <v>19.165833333333335</v>
       </c>
@@ -689,27 +686,27 @@
         <v>25</v>
       </c>
       <c r="F7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="5">
+        <v>0</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="6">
-        <v>0</v>
-      </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" t="s">
         <v>31</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="F8" t="s">
         <v>33</v>
-      </c>
-      <c r="F8" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update tech costs and screenshot to include clerk and totatls
</commit_message>
<xml_diff>
--- a/costs/Tech_costs.xlsx
+++ b/costs/Tech_costs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\tyler\projects\startup\design-and-architecture\costs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE69CCC3-556A-42AF-9262-9C5F8A1F9999}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62E9849F-D0BF-4B4A-8324-3B5BAA7E2C04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-24110" yWindow="-1470" windowWidth="24220" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
   <si>
     <t>Service</t>
   </si>
@@ -147,6 +147,24 @@
   </si>
   <si>
     <t>est. 10,000 visitors month</t>
+  </si>
+  <si>
+    <t>Social Logins</t>
+  </si>
+  <si>
+    <t>Clerk</t>
+  </si>
+  <si>
+    <t>$25 after 10,000 monthly users</t>
+  </si>
+  <si>
+    <t>https://clerk.com/pricing</t>
+  </si>
+  <si>
+    <t>10,000/ Users a month</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -186,7 +204,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -197,6 +215,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF4F81BD"/>
         <bgColor rgb="FF4F81BD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -213,7 +243,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -229,6 +259,8 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -532,10 +564,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -709,6 +741,35 @@
         <v>33</v>
       </c>
     </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="5">
+        <v>0</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="8">
+        <f>SUM(B1:B9)</f>
+        <v>102.16583333333334</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E5" r:id="rId1" xr:uid="{46CAFD59-F628-4100-9708-5A474326D437}"/>
@@ -718,6 +779,7 @@
     <hyperlink ref="E6" r:id="rId5" xr:uid="{6166EEA8-368C-44D5-A8D8-99CD095466C7}"/>
     <hyperlink ref="E7" r:id="rId6" xr:uid="{EC9FC480-53EC-427F-A4B4-9C157AC711AC}"/>
     <hyperlink ref="E8" r:id="rId7" xr:uid="{9DBB71F4-C81E-498C-AF62-FFAB6D366ECD}"/>
+    <hyperlink ref="E9" r:id="rId8" xr:uid="{2FDBB559-95F2-42EA-BF11-A7DDB32C18E5}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>